<commit_message>
Update schedule on redesign
</commit_message>
<xml_diff>
--- a/content/upcoming-conference/ICRAT_2022_Schedule_v8.xlsx
+++ b/content/upcoming-conference/ICRAT_2022_Schedule_v8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Conferences\ICRAT\2022 Tampa\Program Committee\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088811D9-5D53-41FE-89EC-F7D75A481EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CABBDD1-F3AB-402A-BC0D-610D41BCBAB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="270">
   <si>
     <t>Break</t>
   </si>
@@ -836,12 +836,6 @@
     <t>Ryan Graves, Quantum Technology Program Manager, Quantum Generative Materials: Mitigating barriers to the scientific study of Unidentified Aerial Phenomena (UAP): Human Factor considerations of reporting UAP</t>
   </si>
   <si>
-    <t>ICRAT 2022 Conference Schedule (v0.7)</t>
-  </si>
-  <si>
-    <t>Plenary Talk: Bastien Bernard, Director of Operations, Paris Charles de Gaulle Airport:  Airport Future: Becoming Intermodality Node &amp; Energy Hub</t>
-  </si>
-  <si>
     <t>Gala Dinner - Tampa Club (101 E Kennedy Blvd #4200, Tampa, FL 33602) - shuttles will be available from the conference hotels, departing at 5:20 PM</t>
   </si>
   <si>
@@ -849,6 +843,16 @@
   </si>
   <si>
     <t>Doctoral paper sessions 3:50 - 5:10 pm</t>
+  </si>
+  <si>
+    <t>ICRAT 2022 Conference Schedule (v0.8)</t>
+  </si>
+  <si>
+    <t>Plenary Talk: Bastien Bernard, Director of Operations, Paris Charles de Gaulle Airport:  Airport Future: Becoming Intermodality Node &amp; Energy Hub
+and Alex Heiter, Tampa International Airport Director of Research and Air Service Development: Expanding the service network and welcoming the recovery of air industry in post-pandemic era</t>
+  </si>
+  <si>
+    <t>Sign-in 8:30 - 9:00 am</t>
   </si>
 </sst>
 </file>
@@ -1598,7 +1602,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="301">
+  <cellXfs count="299">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1963,7 +1967,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="32" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1973,18 +1976,6 @@
     <xf numFmtId="0" fontId="20" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="35" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2000,12 +1991,6 @@
     <xf numFmtId="0" fontId="35" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="35" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2027,25 +2012,125 @@
     <xf numFmtId="0" fontId="38" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="38" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="20" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="18" fontId="6" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="38" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="13" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2057,61 +2142,83 @@
     <xf numFmtId="0" fontId="37" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="34" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2143,140 +2250,106 @@
     <xf numFmtId="0" fontId="32" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="32" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="11" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="18" fontId="6" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2303,24 +2376,6 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2343,63 +2398,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="9" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="9" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="9" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2419,12 +2417,12 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCCE9AD"/>
       <color rgb="FFF2DCDB"/>
       <color rgb="FF99FF99"/>
       <color rgb="FFFECBA0"/>
       <color rgb="FFDDD9C4"/>
       <color rgb="FFCC8800"/>
-      <color rgb="FFCCE9AD"/>
       <color rgb="FF996600"/>
       <color rgb="FFF8FDB1"/>
       <color rgb="FFEEEAE6"/>
@@ -2734,8 +2732,8 @@
   </sheetPr>
   <dimension ref="A1:P99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42:J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2761,79 +2759,79 @@
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
-      <c r="B1" s="201" t="s">
-        <v>264</v>
-      </c>
-      <c r="C1" s="201"/>
-      <c r="D1" s="201"/>
-      <c r="E1" s="201"/>
-      <c r="F1" s="201"/>
-      <c r="G1" s="201"/>
-      <c r="H1" s="201"/>
-      <c r="I1" s="201"/>
-      <c r="J1" s="201"/>
+      <c r="B1" s="236" t="s">
+        <v>267</v>
+      </c>
+      <c r="C1" s="236"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
+      <c r="F1" s="236"/>
+      <c r="G1" s="236"/>
+      <c r="H1" s="236"/>
+      <c r="I1" s="236"/>
+      <c r="J1" s="236"/>
       <c r="K1" s="22"/>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33"/>
-      <c r="B2" s="202" t="s">
+      <c r="B2" s="237" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="202"/>
-      <c r="D2" s="202"/>
-      <c r="E2" s="203"/>
-      <c r="F2" s="203"/>
-      <c r="G2" s="203"/>
-      <c r="H2" s="203"/>
-      <c r="I2" s="203"/>
-      <c r="J2" s="203"/>
+      <c r="C2" s="237"/>
+      <c r="D2" s="237"/>
+      <c r="E2" s="238"/>
+      <c r="F2" s="238"/>
+      <c r="G2" s="238"/>
+      <c r="H2" s="238"/>
+      <c r="I2" s="238"/>
+      <c r="J2" s="238"/>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="35"/>
-      <c r="B3" s="179" t="s">
+      <c r="B3" s="206" t="s">
         <v>209</v>
       </c>
-      <c r="C3" s="180"/>
-      <c r="D3" s="180"/>
-      <c r="E3" s="180"/>
-      <c r="F3" s="180"/>
-      <c r="G3" s="180"/>
-      <c r="H3" s="180"/>
-      <c r="I3" s="180"/>
-      <c r="J3" s="181"/>
+      <c r="C3" s="207"/>
+      <c r="D3" s="207"/>
+      <c r="E3" s="207"/>
+      <c r="F3" s="207"/>
+      <c r="G3" s="207"/>
+      <c r="H3" s="207"/>
+      <c r="I3" s="207"/>
+      <c r="J3" s="208"/>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="140">
         <v>0.77083333333333337</v>
       </c>
-      <c r="B4" s="204" t="s">
+      <c r="B4" s="239" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="204"/>
-      <c r="D4" s="204"/>
-      <c r="E4" s="204"/>
-      <c r="F4" s="204"/>
-      <c r="G4" s="204"/>
-      <c r="H4" s="204"/>
-      <c r="I4" s="205"/>
-      <c r="J4" s="205"/>
+      <c r="C4" s="239"/>
+      <c r="D4" s="239"/>
+      <c r="E4" s="239"/>
+      <c r="F4" s="239"/>
+      <c r="G4" s="239"/>
+      <c r="H4" s="239"/>
+      <c r="I4" s="240"/>
+      <c r="J4" s="240"/>
       <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11" s="1" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="140"/>
-      <c r="B5" s="216" t="s">
+      <c r="B5" s="247" t="s">
         <v>69</v>
       </c>
-      <c r="C5" s="216"/>
-      <c r="D5" s="216"/>
-      <c r="E5" s="216"/>
-      <c r="F5" s="216"/>
-      <c r="G5" s="216"/>
-      <c r="H5" s="216"/>
-      <c r="I5" s="216"/>
-      <c r="J5" s="216"/>
+      <c r="C5" s="247"/>
+      <c r="D5" s="247"/>
+      <c r="E5" s="247"/>
+      <c r="F5" s="247"/>
+      <c r="G5" s="247"/>
+      <c r="H5" s="247"/>
+      <c r="I5" s="247"/>
+      <c r="J5" s="247"/>
       <c r="K5" s="5"/>
     </row>
     <row r="6" spans="1:11" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -2877,94 +2875,94 @@
     </row>
     <row r="9" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11"/>
-      <c r="B9" s="208" t="s">
+      <c r="B9" s="243" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="208"/>
-      <c r="D9" s="208"/>
-      <c r="E9" s="209"/>
-      <c r="F9" s="209"/>
-      <c r="G9" s="209"/>
-      <c r="H9" s="209"/>
-      <c r="I9" s="209"/>
-      <c r="J9" s="209"/>
+      <c r="C9" s="243"/>
+      <c r="D9" s="243"/>
+      <c r="E9" s="244"/>
+      <c r="F9" s="244"/>
+      <c r="G9" s="244"/>
+      <c r="H9" s="244"/>
+      <c r="I9" s="244"/>
+      <c r="J9" s="244"/>
       <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>0.34375</v>
       </c>
-      <c r="B10" s="206" t="s">
+      <c r="B10" s="241" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="206"/>
-      <c r="D10" s="206"/>
-      <c r="E10" s="206"/>
-      <c r="F10" s="206"/>
-      <c r="G10" s="206"/>
-      <c r="H10" s="206"/>
-      <c r="I10" s="207"/>
-      <c r="J10" s="207"/>
+      <c r="C10" s="241"/>
+      <c r="D10" s="241"/>
+      <c r="E10" s="241"/>
+      <c r="F10" s="241"/>
+      <c r="G10" s="241"/>
+      <c r="H10" s="241"/>
+      <c r="I10" s="242"/>
+      <c r="J10" s="242"/>
       <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:11" s="1" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="35"/>
-      <c r="B11" s="179" t="s">
+      <c r="B11" s="206" t="s">
         <v>195</v>
       </c>
-      <c r="C11" s="180"/>
-      <c r="D11" s="180"/>
-      <c r="E11" s="180"/>
-      <c r="F11" s="180"/>
-      <c r="G11" s="180"/>
-      <c r="H11" s="180"/>
-      <c r="I11" s="180"/>
-      <c r="J11" s="181"/>
+      <c r="C11" s="207"/>
+      <c r="D11" s="207"/>
+      <c r="E11" s="207"/>
+      <c r="F11" s="207"/>
+      <c r="G11" s="207"/>
+      <c r="H11" s="207"/>
+      <c r="I11" s="207"/>
+      <c r="J11" s="208"/>
       <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:11" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
         <v>0.38541666666666669</v>
       </c>
-      <c r="B12" s="211" t="s">
+      <c r="B12" s="246" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="212"/>
-      <c r="D12" s="212"/>
-      <c r="E12" s="212"/>
-      <c r="F12" s="212"/>
-      <c r="G12" s="212"/>
-      <c r="H12" s="212"/>
-      <c r="I12" s="212"/>
-      <c r="J12" s="212"/>
+      <c r="C12" s="227"/>
+      <c r="D12" s="227"/>
+      <c r="E12" s="227"/>
+      <c r="F12" s="227"/>
+      <c r="G12" s="227"/>
+      <c r="H12" s="227"/>
+      <c r="I12" s="227"/>
+      <c r="J12" s="227"/>
       <c r="K12" s="34"/>
     </row>
     <row r="13" spans="1:11" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
         <v>0.3923611111111111</v>
       </c>
-      <c r="B13" s="210" t="s">
+      <c r="B13" s="245" t="s">
         <v>150</v>
       </c>
-      <c r="C13" s="210"/>
-      <c r="D13" s="210"/>
-      <c r="E13" s="210"/>
-      <c r="F13" s="210"/>
-      <c r="G13" s="210"/>
-      <c r="H13" s="210"/>
-      <c r="I13" s="210"/>
-      <c r="J13" s="210"/>
+      <c r="C13" s="245"/>
+      <c r="D13" s="245"/>
+      <c r="E13" s="245"/>
+      <c r="F13" s="245"/>
+      <c r="G13" s="245"/>
+      <c r="H13" s="245"/>
+      <c r="I13" s="245"/>
+      <c r="J13" s="245"/>
       <c r="K13" s="34"/>
     </row>
     <row r="14" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="233" t="s">
+      <c r="B14" s="205" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="233"/>
-      <c r="D14" s="233"/>
-      <c r="E14" s="233"/>
-      <c r="F14" s="233"/>
-      <c r="G14" s="233"/>
+      <c r="C14" s="205"/>
+      <c r="D14" s="205"/>
+      <c r="E14" s="205"/>
+      <c r="F14" s="205"/>
+      <c r="G14" s="205"/>
       <c r="H14" s="92"/>
       <c r="I14" s="92"/>
       <c r="J14" s="92"/>
@@ -2972,36 +2970,36 @@
     </row>
     <row r="15" spans="1:11" s="1" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="35"/>
-      <c r="B15" s="191" t="s">
+      <c r="B15" s="201" t="s">
         <v>196</v>
       </c>
-      <c r="C15" s="192"/>
-      <c r="D15" s="192"/>
-      <c r="E15" s="191" t="s">
+      <c r="C15" s="202"/>
+      <c r="D15" s="202"/>
+      <c r="E15" s="201" t="s">
         <v>197</v>
       </c>
-      <c r="F15" s="192"/>
-      <c r="G15" s="192"/>
+      <c r="F15" s="202"/>
+      <c r="G15" s="202"/>
       <c r="H15" s="93"/>
       <c r="I15" s="94"/>
       <c r="J15" s="94"/>
     </row>
-    <row r="16" spans="1:11" s="9" customFormat="1" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" s="9" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14">
         <v>0.40625</v>
       </c>
-      <c r="B16" s="235" t="s">
+      <c r="B16" s="203" t="s">
         <v>227</v>
       </c>
-      <c r="C16" s="236"/>
-      <c r="D16" s="171" t="s">
+      <c r="C16" s="204"/>
+      <c r="D16" s="164" t="s">
         <v>228</v>
       </c>
-      <c r="E16" s="235" t="s">
+      <c r="E16" s="203" t="s">
         <v>239</v>
       </c>
-      <c r="F16" s="236"/>
-      <c r="G16" s="172" t="s">
+      <c r="F16" s="204"/>
+      <c r="G16" s="173" t="s">
         <v>235</v>
       </c>
       <c r="H16" s="62"/>
@@ -3013,32 +3011,32 @@
       <c r="A17" s="13">
         <v>0.44791666666666669</v>
       </c>
-      <c r="B17" s="213" t="s">
+      <c r="B17" s="210" t="s">
         <v>200</v>
       </c>
-      <c r="C17" s="213"/>
-      <c r="D17" s="213"/>
-      <c r="E17" s="213"/>
-      <c r="F17" s="213"/>
-      <c r="G17" s="213"/>
-      <c r="H17" s="213"/>
-      <c r="I17" s="214"/>
-      <c r="J17" s="214"/>
+      <c r="C17" s="210"/>
+      <c r="D17" s="210"/>
+      <c r="E17" s="210"/>
+      <c r="F17" s="210"/>
+      <c r="G17" s="210"/>
+      <c r="H17" s="210"/>
+      <c r="I17" s="211"/>
+      <c r="J17" s="211"/>
       <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:15" s="1" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
-      <c r="B18" s="215" t="s">
+      <c r="B18" s="231" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="215"/>
-      <c r="D18" s="215"/>
-      <c r="E18" s="215"/>
-      <c r="F18" s="215"/>
-      <c r="G18" s="215"/>
-      <c r="H18" s="215"/>
-      <c r="I18" s="215"/>
-      <c r="J18" s="215"/>
+      <c r="C18" s="231"/>
+      <c r="D18" s="231"/>
+      <c r="E18" s="231"/>
+      <c r="F18" s="231"/>
+      <c r="G18" s="231"/>
+      <c r="H18" s="231"/>
+      <c r="I18" s="231"/>
+      <c r="J18" s="231"/>
       <c r="K18" s="37"/>
       <c r="L18" s="37"/>
       <c r="M18" s="27"/>
@@ -3047,63 +3045,63 @@
     </row>
     <row r="19" spans="1:15" s="1" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="35"/>
-      <c r="B19" s="191" t="s">
+      <c r="B19" s="201" t="s">
         <v>196</v>
       </c>
-      <c r="C19" s="192"/>
-      <c r="D19" s="192"/>
-      <c r="E19" s="191" t="s">
+      <c r="C19" s="202"/>
+      <c r="D19" s="202"/>
+      <c r="E19" s="201" t="s">
         <v>197</v>
       </c>
-      <c r="F19" s="192"/>
-      <c r="G19" s="192"/>
-      <c r="H19" s="191" t="s">
+      <c r="F19" s="202"/>
+      <c r="G19" s="202"/>
+      <c r="H19" s="201" t="s">
         <v>198</v>
       </c>
-      <c r="I19" s="192"/>
-      <c r="J19" s="192"/>
+      <c r="I19" s="202"/>
+      <c r="J19" s="209"/>
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:15" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="13"/>
-      <c r="B20" s="188" t="s">
+      <c r="B20" s="185" t="s">
         <v>83</v>
       </c>
-      <c r="C20" s="189"/>
-      <c r="D20" s="189"/>
-      <c r="E20" s="188" t="s">
+      <c r="C20" s="186"/>
+      <c r="D20" s="186"/>
+      <c r="E20" s="185" t="s">
         <v>74</v>
       </c>
-      <c r="F20" s="189"/>
-      <c r="G20" s="189"/>
-      <c r="H20" s="188" t="s">
+      <c r="F20" s="186"/>
+      <c r="G20" s="186"/>
+      <c r="H20" s="185" t="s">
         <v>77</v>
       </c>
-      <c r="I20" s="189"/>
-      <c r="J20" s="190"/>
+      <c r="I20" s="186"/>
+      <c r="J20" s="253"/>
       <c r="K20" s="42"/>
       <c r="L20" s="37"/>
-      <c r="M20" s="176"/>
-      <c r="N20" s="176"/>
-      <c r="O20" s="176"/>
+      <c r="M20" s="250"/>
+      <c r="N20" s="250"/>
+      <c r="O20" s="250"/>
     </row>
     <row r="21" spans="1:15" s="1" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
-      <c r="B21" s="177" t="s">
+      <c r="B21" s="187" t="s">
         <v>213</v>
       </c>
-      <c r="C21" s="178"/>
-      <c r="D21" s="178"/>
-      <c r="E21" s="177" t="s">
+      <c r="C21" s="188"/>
+      <c r="D21" s="188"/>
+      <c r="E21" s="187" t="s">
         <v>214</v>
       </c>
-      <c r="F21" s="178"/>
-      <c r="G21" s="178"/>
-      <c r="H21" s="177" t="s">
+      <c r="F21" s="188"/>
+      <c r="G21" s="188"/>
+      <c r="H21" s="187" t="s">
         <v>212</v>
       </c>
-      <c r="I21" s="178"/>
-      <c r="J21" s="178"/>
+      <c r="I21" s="188"/>
+      <c r="J21" s="188"/>
       <c r="K21" s="42"/>
       <c r="L21" s="37"/>
       <c r="M21" s="36"/>
@@ -3180,9 +3178,9 @@
       </c>
       <c r="K23" s="42"/>
       <c r="L23" s="37"/>
-      <c r="M23" s="176"/>
-      <c r="N23" s="176"/>
-      <c r="O23" s="176"/>
+      <c r="M23" s="250"/>
+      <c r="N23" s="250"/>
+      <c r="O23" s="250"/>
     </row>
     <row r="24" spans="1:15" s="1" customFormat="1" ht="53.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14">
@@ -3225,124 +3223,124 @@
       <c r="A25" s="16">
         <v>0.55208333333333337</v>
       </c>
-      <c r="B25" s="198" t="s">
+      <c r="B25" s="179" t="s">
         <v>199</v>
       </c>
-      <c r="C25" s="198"/>
-      <c r="D25" s="198"/>
-      <c r="E25" s="198"/>
-      <c r="F25" s="198"/>
-      <c r="G25" s="198"/>
-      <c r="H25" s="224"/>
-      <c r="I25" s="224"/>
-      <c r="J25" s="224"/>
+      <c r="C25" s="179"/>
+      <c r="D25" s="179"/>
+      <c r="E25" s="179"/>
+      <c r="F25" s="179"/>
+      <c r="G25" s="179"/>
+      <c r="H25" s="226"/>
+      <c r="I25" s="226"/>
+      <c r="J25" s="226"/>
       <c r="K25" s="37"/>
       <c r="L25" s="37"/>
-      <c r="M25" s="176"/>
-      <c r="N25" s="176"/>
-      <c r="O25" s="176"/>
+      <c r="M25" s="250"/>
+      <c r="N25" s="250"/>
+      <c r="O25" s="250"/>
     </row>
     <row r="26" spans="1:15" s="1" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="35"/>
-      <c r="B26" s="179" t="s">
+      <c r="B26" s="206" t="s">
         <v>195</v>
       </c>
-      <c r="C26" s="180"/>
-      <c r="D26" s="180"/>
-      <c r="E26" s="180"/>
-      <c r="F26" s="180"/>
-      <c r="G26" s="180"/>
-      <c r="H26" s="180"/>
-      <c r="I26" s="180"/>
-      <c r="J26" s="181"/>
+      <c r="C26" s="207"/>
+      <c r="D26" s="207"/>
+      <c r="E26" s="207"/>
+      <c r="F26" s="207"/>
+      <c r="G26" s="207"/>
+      <c r="H26" s="207"/>
+      <c r="I26" s="207"/>
+      <c r="J26" s="208"/>
       <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:15" s="31" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="16">
         <v>0.59375</v>
       </c>
-      <c r="B27" s="211" t="s">
+      <c r="B27" s="246" t="s">
         <v>262</v>
       </c>
-      <c r="C27" s="211"/>
-      <c r="D27" s="211"/>
-      <c r="E27" s="211"/>
-      <c r="F27" s="211"/>
-      <c r="G27" s="211"/>
-      <c r="H27" s="211"/>
-      <c r="I27" s="217"/>
-      <c r="J27" s="217"/>
+      <c r="C27" s="246"/>
+      <c r="D27" s="246"/>
+      <c r="E27" s="246"/>
+      <c r="F27" s="246"/>
+      <c r="G27" s="246"/>
+      <c r="H27" s="246"/>
+      <c r="I27" s="248"/>
+      <c r="J27" s="248"/>
       <c r="K27" s="29"/>
     </row>
     <row r="28" spans="1:15" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
         <v>0.63541666666666663</v>
       </c>
-      <c r="B28" s="199" t="s">
+      <c r="B28" s="189" t="s">
         <v>201</v>
       </c>
-      <c r="C28" s="199"/>
-      <c r="D28" s="199"/>
-      <c r="E28" s="199"/>
-      <c r="F28" s="199"/>
-      <c r="G28" s="199"/>
-      <c r="H28" s="199"/>
-      <c r="I28" s="199"/>
-      <c r="J28" s="199"/>
+      <c r="C28" s="189"/>
+      <c r="D28" s="189"/>
+      <c r="E28" s="189"/>
+      <c r="F28" s="189"/>
+      <c r="G28" s="189"/>
+      <c r="H28" s="189"/>
+      <c r="I28" s="189"/>
+      <c r="J28" s="189"/>
       <c r="K28" s="2"/>
       <c r="L28"/>
     </row>
     <row r="29" spans="1:15" s="1" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="13"/>
-      <c r="B29" s="215" t="s">
+      <c r="B29" s="231" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="215"/>
-      <c r="D29" s="215"/>
-      <c r="E29" s="215"/>
-      <c r="F29" s="215"/>
-      <c r="G29" s="215"/>
-      <c r="H29" s="215"/>
-      <c r="I29" s="215"/>
-      <c r="J29" s="215"/>
+      <c r="C29" s="231"/>
+      <c r="D29" s="231"/>
+      <c r="E29" s="231"/>
+      <c r="F29" s="231"/>
+      <c r="G29" s="231"/>
+      <c r="H29" s="231"/>
+      <c r="I29" s="231"/>
+      <c r="J29" s="231"/>
       <c r="K29" s="2"/>
       <c r="L29" s="17"/>
     </row>
     <row r="30" spans="1:15" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="188" t="s">
+      <c r="B30" s="185" t="s">
         <v>75</v>
       </c>
-      <c r="C30" s="189"/>
-      <c r="D30" s="189"/>
-      <c r="E30" s="188" t="s">
+      <c r="C30" s="186"/>
+      <c r="D30" s="186"/>
+      <c r="E30" s="185" t="s">
         <v>76</v>
       </c>
-      <c r="F30" s="189"/>
-      <c r="G30" s="189"/>
-      <c r="H30" s="188" t="s">
+      <c r="F30" s="186"/>
+      <c r="G30" s="186"/>
+      <c r="H30" s="185" t="s">
         <v>78</v>
       </c>
-      <c r="I30" s="189"/>
-      <c r="J30" s="189"/>
+      <c r="I30" s="186"/>
+      <c r="J30" s="186"/>
       <c r="K30" s="43"/>
       <c r="L30"/>
     </row>
     <row r="31" spans="1:15" s="1" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="177" t="s">
+      <c r="B31" s="187" t="s">
         <v>218</v>
       </c>
-      <c r="C31" s="178"/>
-      <c r="D31" s="178"/>
-      <c r="E31" s="177" t="s">
+      <c r="C31" s="188"/>
+      <c r="D31" s="188"/>
+      <c r="E31" s="187" t="s">
         <v>224</v>
       </c>
-      <c r="F31" s="178"/>
-      <c r="G31" s="178"/>
-      <c r="H31" s="177" t="s">
+      <c r="F31" s="188"/>
+      <c r="G31" s="188"/>
+      <c r="H31" s="187" t="s">
         <v>223</v>
       </c>
-      <c r="I31" s="178"/>
-      <c r="J31" s="178"/>
+      <c r="I31" s="188"/>
+      <c r="J31" s="188"/>
       <c r="K31" s="43"/>
       <c r="L31"/>
     </row>
@@ -3379,9 +3377,9 @@
       </c>
       <c r="K32" s="44"/>
       <c r="L32" s="20"/>
-      <c r="M32" s="182"/>
-      <c r="N32" s="182"/>
-      <c r="O32" s="182"/>
+      <c r="M32" s="251"/>
+      <c r="N32" s="251"/>
+      <c r="O32" s="251"/>
     </row>
     <row r="33" spans="1:15" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="14">
@@ -3454,17 +3452,17 @@
       <c r="A35" s="13">
         <v>0.73958333333333337</v>
       </c>
-      <c r="B35" s="198" t="s">
+      <c r="B35" s="179" t="s">
         <v>0</v>
       </c>
-      <c r="C35" s="198"/>
-      <c r="D35" s="198"/>
-      <c r="E35" s="198"/>
-      <c r="F35" s="198"/>
-      <c r="G35" s="198"/>
-      <c r="H35" s="198"/>
-      <c r="I35" s="198"/>
-      <c r="J35" s="198"/>
+      <c r="C35" s="179"/>
+      <c r="D35" s="179"/>
+      <c r="E35" s="179"/>
+      <c r="F35" s="179"/>
+      <c r="G35" s="179"/>
+      <c r="H35" s="179"/>
+      <c r="I35" s="179"/>
+      <c r="J35" s="179"/>
       <c r="K35" s="5"/>
       <c r="L35"/>
     </row>
@@ -3509,66 +3507,66 @@
     </row>
     <row r="39" spans="1:15" s="1" customFormat="1" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A39" s="33"/>
-      <c r="B39" s="227" t="s">
+      <c r="B39" s="180" t="s">
         <v>63</v>
       </c>
-      <c r="C39" s="227"/>
-      <c r="D39" s="227"/>
-      <c r="E39" s="228"/>
-      <c r="F39" s="228"/>
-      <c r="G39" s="228"/>
-      <c r="H39" s="228"/>
-      <c r="I39" s="228"/>
-      <c r="J39" s="228"/>
+      <c r="C39" s="180"/>
+      <c r="D39" s="180"/>
+      <c r="E39" s="230"/>
+      <c r="F39" s="230"/>
+      <c r="G39" s="230"/>
+      <c r="H39" s="230"/>
+      <c r="I39" s="230"/>
+      <c r="J39" s="230"/>
       <c r="K39" s="5"/>
       <c r="L39" s="18"/>
     </row>
     <row r="40" spans="1:15" s="1" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="13">
-        <v>0.36458333333333331</v>
-      </c>
-      <c r="B40" s="238" t="s">
-        <v>152</v>
-      </c>
-      <c r="C40" s="238"/>
-      <c r="D40" s="238"/>
-      <c r="E40" s="238"/>
-      <c r="F40" s="238"/>
-      <c r="G40" s="238"/>
-      <c r="H40" s="238"/>
-      <c r="I40" s="239"/>
-      <c r="J40" s="239"/>
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="B40" s="212" t="s">
+        <v>269</v>
+      </c>
+      <c r="C40" s="212"/>
+      <c r="D40" s="212"/>
+      <c r="E40" s="212"/>
+      <c r="F40" s="212"/>
+      <c r="G40" s="212"/>
+      <c r="H40" s="212"/>
+      <c r="I40" s="213"/>
+      <c r="J40" s="213"/>
     </row>
     <row r="41" spans="1:15" s="1" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="35"/>
-      <c r="B41" s="179" t="s">
+      <c r="B41" s="206" t="s">
         <v>195</v>
       </c>
-      <c r="C41" s="180"/>
-      <c r="D41" s="180"/>
-      <c r="E41" s="180"/>
-      <c r="F41" s="180"/>
-      <c r="G41" s="180"/>
-      <c r="H41" s="180"/>
-      <c r="I41" s="180"/>
-      <c r="J41" s="181"/>
+      <c r="C41" s="207"/>
+      <c r="D41" s="207"/>
+      <c r="E41" s="207"/>
+      <c r="F41" s="207"/>
+      <c r="G41" s="207"/>
+      <c r="H41" s="207"/>
+      <c r="I41" s="207"/>
+      <c r="J41" s="208"/>
       <c r="K41" s="2"/>
     </row>
     <row r="42" spans="1:15" s="31" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="14">
-        <v>0.38541666666666669</v>
-      </c>
-      <c r="B42" s="212" t="s">
-        <v>265</v>
-      </c>
-      <c r="C42" s="212"/>
-      <c r="D42" s="212"/>
-      <c r="E42" s="212"/>
-      <c r="F42" s="212"/>
-      <c r="G42" s="212"/>
-      <c r="H42" s="212"/>
-      <c r="I42" s="218"/>
-      <c r="J42" s="218"/>
+        <v>0.375</v>
+      </c>
+      <c r="B42" s="246" t="s">
+        <v>268</v>
+      </c>
+      <c r="C42" s="246"/>
+      <c r="D42" s="246"/>
+      <c r="E42" s="246"/>
+      <c r="F42" s="246"/>
+      <c r="G42" s="246"/>
+      <c r="H42" s="246"/>
+      <c r="I42" s="248"/>
+      <c r="J42" s="248"/>
       <c r="K42" s="29"/>
       <c r="L42" s="32"/>
     </row>
@@ -3576,77 +3574,77 @@
       <c r="A43" s="13">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B43" s="213" t="s">
+      <c r="B43" s="210" t="s">
         <v>206</v>
       </c>
-      <c r="C43" s="213"/>
-      <c r="D43" s="213"/>
-      <c r="E43" s="213"/>
-      <c r="F43" s="213"/>
-      <c r="G43" s="213"/>
-      <c r="H43" s="213"/>
-      <c r="I43" s="214"/>
-      <c r="J43" s="214"/>
+      <c r="C43" s="210"/>
+      <c r="D43" s="210"/>
+      <c r="E43" s="210"/>
+      <c r="F43" s="210"/>
+      <c r="G43" s="210"/>
+      <c r="H43" s="210"/>
+      <c r="I43" s="211"/>
+      <c r="J43" s="211"/>
       <c r="K43" s="2"/>
       <c r="L43" s="18"/>
     </row>
     <row r="44" spans="1:15" s="1" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="233" t="s">
+      <c r="B44" s="205" t="s">
         <v>19</v>
       </c>
-      <c r="C44" s="233"/>
-      <c r="D44" s="233"/>
-      <c r="E44" s="233"/>
-      <c r="F44" s="233"/>
-      <c r="G44" s="233"/>
-      <c r="H44" s="233"/>
-      <c r="I44" s="233"/>
-      <c r="J44" s="233"/>
+      <c r="C44" s="205"/>
+      <c r="D44" s="205"/>
+      <c r="E44" s="205"/>
+      <c r="F44" s="205"/>
+      <c r="G44" s="205"/>
+      <c r="H44" s="205"/>
+      <c r="I44" s="205"/>
+      <c r="J44" s="205"/>
       <c r="K44" s="5"/>
       <c r="L44"/>
     </row>
     <row r="45" spans="1:15" s="1" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="35"/>
-      <c r="B45" s="191" t="s">
+      <c r="B45" s="201" t="s">
         <v>203</v>
       </c>
-      <c r="C45" s="192"/>
-      <c r="D45" s="192"/>
-      <c r="E45" s="191" t="s">
+      <c r="C45" s="202"/>
+      <c r="D45" s="202"/>
+      <c r="E45" s="201" t="s">
         <v>204</v>
       </c>
-      <c r="F45" s="192"/>
-      <c r="G45" s="192"/>
-      <c r="H45" s="191" t="s">
+      <c r="F45" s="202"/>
+      <c r="G45" s="202"/>
+      <c r="H45" s="201" t="s">
         <v>202</v>
       </c>
-      <c r="I45" s="192"/>
-      <c r="J45" s="237"/>
+      <c r="I45" s="202"/>
+      <c r="J45" s="209"/>
       <c r="K45" s="2"/>
     </row>
     <row r="46" spans="1:15" s="1" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="41">
         <v>0.4375</v>
       </c>
-      <c r="B46" s="183" t="s">
+      <c r="B46" s="199" t="s">
         <v>229</v>
       </c>
-      <c r="C46" s="184"/>
-      <c r="D46" s="173" t="s">
+      <c r="C46" s="200"/>
+      <c r="D46" s="165" t="s">
         <v>230</v>
       </c>
-      <c r="E46" s="183" t="s">
+      <c r="E46" s="199" t="s">
         <v>236</v>
       </c>
-      <c r="F46" s="184"/>
-      <c r="G46" s="173" t="s">
+      <c r="F46" s="200"/>
+      <c r="G46" s="165" t="s">
         <v>232</v>
       </c>
-      <c r="H46" s="183" t="s">
+      <c r="H46" s="199" t="s">
         <v>233</v>
       </c>
-      <c r="I46" s="184"/>
-      <c r="J46" s="174" t="s">
+      <c r="I46" s="200"/>
+      <c r="J46" s="166" t="s">
         <v>234</v>
       </c>
       <c r="K46" s="40"/>
@@ -3659,17 +3657,17 @@
       <c r="A47" s="15">
         <v>0.52083333333333337</v>
       </c>
-      <c r="B47" s="198" t="s">
+      <c r="B47" s="179" t="s">
         <v>205</v>
       </c>
-      <c r="C47" s="198"/>
-      <c r="D47" s="198"/>
-      <c r="E47" s="198"/>
-      <c r="F47" s="198"/>
-      <c r="G47" s="198"/>
-      <c r="H47" s="198"/>
-      <c r="I47" s="198"/>
-      <c r="J47" s="198"/>
+      <c r="C47" s="179"/>
+      <c r="D47" s="179"/>
+      <c r="E47" s="179"/>
+      <c r="F47" s="179"/>
+      <c r="G47" s="179"/>
+      <c r="H47" s="179"/>
+      <c r="I47" s="179"/>
+      <c r="J47" s="179"/>
       <c r="K47" s="5"/>
       <c r="L47" s="91"/>
       <c r="M47" s="91"/>
@@ -3716,17 +3714,17 @@
     </row>
     <row r="51" spans="1:16" s="52" customFormat="1" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A51" s="33"/>
-      <c r="B51" s="227" t="s">
+      <c r="B51" s="180" t="s">
         <v>64</v>
       </c>
-      <c r="C51" s="227"/>
-      <c r="D51" s="227"/>
-      <c r="E51" s="228"/>
-      <c r="F51" s="228"/>
-      <c r="G51" s="228"/>
-      <c r="H51" s="228"/>
-      <c r="I51" s="228"/>
-      <c r="J51" s="228"/>
+      <c r="C51" s="180"/>
+      <c r="D51" s="180"/>
+      <c r="E51" s="230"/>
+      <c r="F51" s="230"/>
+      <c r="G51" s="230"/>
+      <c r="H51" s="230"/>
+      <c r="I51" s="230"/>
+      <c r="J51" s="230"/>
       <c r="K51" s="60"/>
       <c r="L51" s="61"/>
     </row>
@@ -3734,50 +3732,50 @@
       <c r="A52" s="13">
         <v>0.36458333333333331</v>
       </c>
-      <c r="B52" s="238" t="s">
+      <c r="B52" s="212" t="s">
         <v>152</v>
       </c>
-      <c r="C52" s="238"/>
-      <c r="D52" s="238"/>
-      <c r="E52" s="238"/>
-      <c r="F52" s="238"/>
-      <c r="G52" s="238"/>
-      <c r="H52" s="238"/>
-      <c r="I52" s="239"/>
-      <c r="J52" s="239"/>
+      <c r="C52" s="212"/>
+      <c r="D52" s="212"/>
+      <c r="E52" s="212"/>
+      <c r="F52" s="212"/>
+      <c r="G52" s="212"/>
+      <c r="H52" s="212"/>
+      <c r="I52" s="213"/>
+      <c r="J52" s="213"/>
       <c r="K52" s="2"/>
       <c r="L52"/>
     </row>
     <row r="53" spans="1:16" s="1" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="35"/>
-      <c r="B53" s="179" t="s">
+      <c r="B53" s="206" t="s">
         <v>195</v>
       </c>
-      <c r="C53" s="180"/>
-      <c r="D53" s="180"/>
-      <c r="E53" s="180"/>
-      <c r="F53" s="180"/>
-      <c r="G53" s="180"/>
-      <c r="H53" s="180"/>
-      <c r="I53" s="180"/>
-      <c r="J53" s="181"/>
+      <c r="C53" s="207"/>
+      <c r="D53" s="207"/>
+      <c r="E53" s="207"/>
+      <c r="F53" s="207"/>
+      <c r="G53" s="207"/>
+      <c r="H53" s="207"/>
+      <c r="I53" s="207"/>
+      <c r="J53" s="208"/>
       <c r="K53" s="2"/>
     </row>
     <row r="54" spans="1:16" s="31" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="14">
         <v>0.38541666666666669</v>
       </c>
-      <c r="B54" s="212" t="s">
+      <c r="B54" s="227" t="s">
         <v>263</v>
       </c>
-      <c r="C54" s="225"/>
-      <c r="D54" s="225"/>
-      <c r="E54" s="225"/>
-      <c r="F54" s="225"/>
-      <c r="G54" s="225"/>
-      <c r="H54" s="225"/>
-      <c r="I54" s="226"/>
-      <c r="J54" s="226"/>
+      <c r="C54" s="228"/>
+      <c r="D54" s="228"/>
+      <c r="E54" s="228"/>
+      <c r="F54" s="228"/>
+      <c r="G54" s="228"/>
+      <c r="H54" s="228"/>
+      <c r="I54" s="229"/>
+      <c r="J54" s="229"/>
       <c r="K54" s="29"/>
       <c r="L54" s="30"/>
     </row>
@@ -3785,76 +3783,76 @@
       <c r="A55" s="13">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B55" s="213" t="s">
+      <c r="B55" s="210" t="s">
         <v>207</v>
       </c>
-      <c r="C55" s="213"/>
-      <c r="D55" s="213"/>
-      <c r="E55" s="213"/>
-      <c r="F55" s="213"/>
-      <c r="G55" s="213"/>
-      <c r="H55" s="213"/>
-      <c r="I55" s="214"/>
-      <c r="J55" s="214"/>
+      <c r="C55" s="210"/>
+      <c r="D55" s="210"/>
+      <c r="E55" s="210"/>
+      <c r="F55" s="210"/>
+      <c r="G55" s="210"/>
+      <c r="H55" s="210"/>
+      <c r="I55" s="211"/>
+      <c r="J55" s="211"/>
       <c r="K55" s="5"/>
       <c r="L55"/>
     </row>
     <row r="56" spans="1:16" s="1" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="242" t="s">
+      <c r="B56" s="218" t="s">
         <v>20</v>
       </c>
-      <c r="C56" s="242"/>
-      <c r="D56" s="242"/>
-      <c r="E56" s="242"/>
-      <c r="F56" s="242"/>
-      <c r="G56" s="242"/>
-      <c r="H56" s="242"/>
-      <c r="I56" s="242"/>
-      <c r="J56" s="242"/>
+      <c r="C56" s="218"/>
+      <c r="D56" s="218"/>
+      <c r="E56" s="218"/>
+      <c r="F56" s="218"/>
+      <c r="G56" s="218"/>
+      <c r="H56" s="218"/>
+      <c r="I56" s="218"/>
+      <c r="J56" s="218"/>
       <c r="K56" s="2"/>
     </row>
     <row r="57" spans="1:16" s="1" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="35"/>
-      <c r="B57" s="191" t="s">
+      <c r="B57" s="201" t="s">
         <v>196</v>
       </c>
-      <c r="C57" s="192"/>
-      <c r="D57" s="192"/>
-      <c r="E57" s="191" t="s">
+      <c r="C57" s="202"/>
+      <c r="D57" s="202"/>
+      <c r="E57" s="201" t="s">
         <v>197</v>
       </c>
-      <c r="F57" s="192"/>
-      <c r="G57" s="192"/>
-      <c r="H57" s="191" t="s">
+      <c r="F57" s="202"/>
+      <c r="G57" s="202"/>
+      <c r="H57" s="201" t="s">
         <v>198</v>
       </c>
-      <c r="I57" s="192"/>
-      <c r="J57" s="192"/>
+      <c r="I57" s="202"/>
+      <c r="J57" s="202"/>
       <c r="K57" s="43"/>
     </row>
     <row r="58" spans="1:16" s="1" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="234">
+      <c r="A58" s="198">
         <v>0.4375</v>
       </c>
-      <c r="B58" s="183" t="s">
+      <c r="B58" s="199" t="s">
         <v>229</v>
       </c>
-      <c r="C58" s="184"/>
-      <c r="D58" s="184" t="s">
+      <c r="C58" s="200"/>
+      <c r="D58" s="200" t="s">
         <v>231</v>
       </c>
-      <c r="E58" s="183" t="s">
+      <c r="E58" s="199" t="s">
         <v>237</v>
       </c>
-      <c r="F58" s="184"/>
-      <c r="G58" s="184" t="s">
+      <c r="F58" s="200"/>
+      <c r="G58" s="200" t="s">
         <v>238</v>
       </c>
-      <c r="H58" s="183" t="s">
+      <c r="H58" s="199" t="s">
         <v>260</v>
       </c>
-      <c r="I58" s="184"/>
-      <c r="J58" s="240" t="s">
+      <c r="I58" s="200"/>
+      <c r="J58" s="216" t="s">
         <v>261</v>
       </c>
       <c r="K58" s="62"/>
@@ -3863,16 +3861,16 @@
       <c r="O58" s="28"/>
     </row>
     <row r="59" spans="1:16" s="1" customFormat="1" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="234"/>
-      <c r="B59" s="243"/>
-      <c r="C59" s="244"/>
-      <c r="D59" s="244"/>
-      <c r="E59" s="185"/>
-      <c r="F59" s="186"/>
-      <c r="G59" s="186"/>
-      <c r="H59" s="185"/>
-      <c r="I59" s="186"/>
-      <c r="J59" s="241"/>
+      <c r="A59" s="198"/>
+      <c r="B59" s="219"/>
+      <c r="C59" s="220"/>
+      <c r="D59" s="220"/>
+      <c r="E59" s="215"/>
+      <c r="F59" s="214"/>
+      <c r="G59" s="214"/>
+      <c r="H59" s="215"/>
+      <c r="I59" s="214"/>
+      <c r="J59" s="217"/>
       <c r="K59" s="62"/>
       <c r="L59" s="62"/>
       <c r="N59" s="10"/>
@@ -3882,32 +3880,32 @@
       <c r="A60" s="15">
         <v>0.52083333333333337</v>
       </c>
-      <c r="B60" s="198" t="s">
+      <c r="B60" s="179" t="s">
         <v>151</v>
       </c>
-      <c r="C60" s="198"/>
-      <c r="D60" s="198"/>
-      <c r="E60" s="198"/>
-      <c r="F60" s="198"/>
-      <c r="G60" s="198"/>
-      <c r="H60" s="198"/>
-      <c r="I60" s="198"/>
-      <c r="J60" s="198"/>
+      <c r="C60" s="179"/>
+      <c r="D60" s="179"/>
+      <c r="E60" s="179"/>
+      <c r="F60" s="179"/>
+      <c r="G60" s="179"/>
+      <c r="H60" s="179"/>
+      <c r="I60" s="179"/>
+      <c r="J60" s="179"/>
       <c r="K60" s="5"/>
     </row>
     <row r="61" spans="1:16" s="1" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
-      <c r="B61" s="215" t="s">
+      <c r="B61" s="231" t="s">
         <v>21</v>
       </c>
-      <c r="C61" s="215"/>
-      <c r="D61" s="215"/>
-      <c r="E61" s="215"/>
-      <c r="F61" s="215"/>
-      <c r="G61" s="215"/>
-      <c r="H61" s="215"/>
-      <c r="I61" s="215"/>
-      <c r="J61" s="215"/>
+      <c r="C61" s="231"/>
+      <c r="D61" s="231"/>
+      <c r="E61" s="231"/>
+      <c r="F61" s="231"/>
+      <c r="G61" s="231"/>
+      <c r="H61" s="231"/>
+      <c r="I61" s="231"/>
+      <c r="J61" s="231"/>
       <c r="K61" s="5"/>
       <c r="L61" s="10"/>
       <c r="M61" s="10"/>
@@ -3917,21 +3915,21 @@
     </row>
     <row r="62" spans="1:16" s="1" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="35"/>
-      <c r="B62" s="191" t="s">
+      <c r="B62" s="201" t="s">
         <v>196</v>
       </c>
-      <c r="C62" s="192"/>
-      <c r="D62" s="192"/>
-      <c r="E62" s="191" t="s">
+      <c r="C62" s="202"/>
+      <c r="D62" s="202"/>
+      <c r="E62" s="201" t="s">
         <v>197</v>
       </c>
-      <c r="F62" s="192"/>
-      <c r="G62" s="192"/>
-      <c r="H62" s="191" t="s">
+      <c r="F62" s="202"/>
+      <c r="G62" s="202"/>
+      <c r="H62" s="201" t="s">
         <v>198</v>
       </c>
-      <c r="I62" s="192"/>
-      <c r="J62" s="192"/>
+      <c r="I62" s="202"/>
+      <c r="J62" s="209"/>
       <c r="K62" s="2"/>
       <c r="L62" s="10"/>
       <c r="M62" s="106"/>
@@ -3941,21 +3939,21 @@
     </row>
     <row r="63" spans="1:16" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="13"/>
-      <c r="B63" s="188" t="s">
+      <c r="B63" s="185" t="s">
         <v>84</v>
       </c>
-      <c r="C63" s="189"/>
-      <c r="D63" s="189"/>
-      <c r="E63" s="188" t="s">
+      <c r="C63" s="186"/>
+      <c r="D63" s="186"/>
+      <c r="E63" s="185" t="s">
         <v>79</v>
       </c>
-      <c r="F63" s="189"/>
-      <c r="G63" s="189"/>
-      <c r="H63" s="188" t="s">
+      <c r="F63" s="186"/>
+      <c r="G63" s="186"/>
+      <c r="H63" s="185" t="s">
         <v>80</v>
       </c>
-      <c r="I63" s="189"/>
-      <c r="J63" s="189"/>
+      <c r="I63" s="186"/>
+      <c r="J63" s="186"/>
       <c r="K63" s="46"/>
       <c r="L63" s="39"/>
       <c r="M63" s="107"/>
@@ -3965,21 +3963,21 @@
     </row>
     <row r="64" spans="1:16" s="1" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="13"/>
-      <c r="B64" s="177" t="s">
+      <c r="B64" s="187" t="s">
         <v>225</v>
       </c>
-      <c r="C64" s="178"/>
-      <c r="D64" s="178"/>
-      <c r="E64" s="177" t="s">
+      <c r="C64" s="188"/>
+      <c r="D64" s="188"/>
+      <c r="E64" s="187" t="s">
         <v>222</v>
       </c>
-      <c r="F64" s="178"/>
-      <c r="G64" s="178"/>
-      <c r="H64" s="177" t="s">
+      <c r="F64" s="188"/>
+      <c r="G64" s="188"/>
+      <c r="H64" s="187" t="s">
         <v>226</v>
       </c>
-      <c r="I64" s="178"/>
-      <c r="J64" s="178"/>
+      <c r="I64" s="188"/>
+      <c r="J64" s="188"/>
       <c r="K64" s="47"/>
       <c r="L64" s="38"/>
       <c r="M64" s="104"/>
@@ -4105,71 +4103,71 @@
       <c r="A68" s="16">
         <v>0.64583333333333337</v>
       </c>
-      <c r="B68" s="199" t="s">
-        <v>267</v>
-      </c>
-      <c r="C68" s="199"/>
-      <c r="D68" s="199"/>
-      <c r="E68" s="199"/>
-      <c r="F68" s="199"/>
-      <c r="G68" s="199"/>
-      <c r="H68" s="199"/>
-      <c r="I68" s="199"/>
-      <c r="J68" s="199"/>
+      <c r="B68" s="189" t="s">
+        <v>265</v>
+      </c>
+      <c r="C68" s="189"/>
+      <c r="D68" s="189"/>
+      <c r="E68" s="189"/>
+      <c r="F68" s="189"/>
+      <c r="G68" s="189"/>
+      <c r="H68" s="189"/>
+      <c r="I68" s="189"/>
+      <c r="J68" s="189"/>
       <c r="K68" s="2"/>
       <c r="L68" s="18"/>
     </row>
     <row r="69" spans="1:16" s="1" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="13"/>
-      <c r="B69" s="187" t="s">
-        <v>268</v>
-      </c>
-      <c r="C69" s="187"/>
-      <c r="D69" s="187"/>
-      <c r="E69" s="187"/>
-      <c r="F69" s="187"/>
-      <c r="G69" s="187"/>
-      <c r="H69" s="187"/>
-      <c r="I69" s="187"/>
-      <c r="J69" s="187"/>
+      <c r="B69" s="252" t="s">
+        <v>266</v>
+      </c>
+      <c r="C69" s="252"/>
+      <c r="D69" s="252"/>
+      <c r="E69" s="252"/>
+      <c r="F69" s="252"/>
+      <c r="G69" s="252"/>
+      <c r="H69" s="252"/>
+      <c r="I69" s="252"/>
+      <c r="J69" s="252"/>
       <c r="K69" s="2"/>
       <c r="L69" s="18"/>
     </row>
     <row r="70" spans="1:16" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B70" s="231" t="s">
+      <c r="B70" s="190" t="s">
         <v>161</v>
       </c>
-      <c r="C70" s="232"/>
-      <c r="D70" s="232"/>
-      <c r="E70" s="231" t="s">
+      <c r="C70" s="191"/>
+      <c r="D70" s="191"/>
+      <c r="E70" s="190" t="s">
         <v>162</v>
       </c>
-      <c r="F70" s="232"/>
-      <c r="G70" s="232"/>
-      <c r="H70" s="231" t="s">
+      <c r="F70" s="191"/>
+      <c r="G70" s="191"/>
+      <c r="H70" s="190" t="s">
         <v>163</v>
       </c>
-      <c r="I70" s="232"/>
-      <c r="J70" s="232"/>
+      <c r="I70" s="191"/>
+      <c r="J70" s="191"/>
       <c r="K70" s="46"/>
       <c r="L70" s="39"/>
     </row>
     <row r="71" spans="1:16" s="1" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="195" t="s">
+      <c r="B71" s="193" t="s">
         <v>210</v>
       </c>
-      <c r="C71" s="196"/>
-      <c r="D71" s="196"/>
-      <c r="E71" s="195" t="s">
+      <c r="C71" s="194"/>
+      <c r="D71" s="194"/>
+      <c r="E71" s="193" t="s">
         <v>215</v>
       </c>
-      <c r="F71" s="196"/>
-      <c r="G71" s="196"/>
-      <c r="H71" s="195" t="s">
+      <c r="F71" s="194"/>
+      <c r="G71" s="194"/>
+      <c r="H71" s="193" t="s">
         <v>221</v>
       </c>
-      <c r="I71" s="196"/>
-      <c r="J71" s="196"/>
+      <c r="I71" s="194"/>
+      <c r="J71" s="194"/>
       <c r="K71" s="43"/>
       <c r="L71"/>
     </row>
@@ -4177,31 +4175,31 @@
       <c r="A72" s="41">
         <v>0.65972222222222221</v>
       </c>
-      <c r="B72" s="152">
+      <c r="B72" s="151">
         <v>16</v>
       </c>
-      <c r="C72" s="158" t="s">
+      <c r="C72" s="153" t="s">
         <v>166</v>
       </c>
-      <c r="D72" s="162" t="s">
+      <c r="D72" s="157" t="s">
         <v>167</v>
       </c>
-      <c r="E72" s="152">
+      <c r="E72" s="151">
         <v>23</v>
       </c>
-      <c r="F72" s="158" t="s">
+      <c r="F72" s="153" t="s">
         <v>170</v>
       </c>
-      <c r="G72" s="161" t="s">
+      <c r="G72" s="156" t="s">
         <v>171</v>
       </c>
-      <c r="H72" s="152">
+      <c r="H72" s="151">
         <v>18</v>
       </c>
-      <c r="I72" s="158" t="s">
+      <c r="I72" s="153" t="s">
         <v>174</v>
       </c>
-      <c r="J72" s="162" t="s">
+      <c r="J72" s="157" t="s">
         <v>175</v>
       </c>
       <c r="K72" s="19"/>
@@ -4215,32 +4213,32 @@
       <c r="A73" s="41">
         <v>0.6875</v>
       </c>
-      <c r="B73" s="153">
+      <c r="B73" s="152">
         <v>44</v>
       </c>
-      <c r="C73" s="159" t="s">
+      <c r="C73" s="154" t="s">
         <v>168</v>
       </c>
-      <c r="D73" s="160" t="s">
+      <c r="D73" s="155" t="s">
         <v>169</v>
       </c>
-      <c r="E73" s="153">
+      <c r="E73" s="152">
         <v>28</v>
       </c>
-      <c r="F73" s="159" t="s">
+      <c r="F73" s="154" t="s">
         <v>172</v>
       </c>
-      <c r="G73" s="159" t="s">
+      <c r="G73" s="154" t="s">
         <v>173</v>
       </c>
-      <c r="H73" s="154">
-        <v>21</v>
-      </c>
-      <c r="I73" s="163" t="s">
-        <v>176</v>
-      </c>
-      <c r="J73" s="164" t="s">
-        <v>177</v>
+      <c r="H73" s="167">
+        <v>25</v>
+      </c>
+      <c r="I73" s="160" t="s">
+        <v>184</v>
+      </c>
+      <c r="J73" s="161" t="s">
+        <v>185</v>
       </c>
       <c r="K73" s="3"/>
       <c r="N73" s="26"/>
@@ -4251,17 +4249,17 @@
       <c r="A74" s="13">
         <v>0.71527777777777779</v>
       </c>
-      <c r="B74" s="198" t="s">
+      <c r="B74" s="179" t="s">
         <v>0</v>
       </c>
-      <c r="C74" s="198"/>
-      <c r="D74" s="198"/>
-      <c r="E74" s="198"/>
-      <c r="F74" s="198"/>
-      <c r="G74" s="198"/>
-      <c r="H74" s="198"/>
-      <c r="I74" s="198"/>
-      <c r="J74" s="198"/>
+      <c r="C74" s="179"/>
+      <c r="D74" s="179"/>
+      <c r="E74" s="179"/>
+      <c r="F74" s="179"/>
+      <c r="G74" s="179"/>
+      <c r="H74" s="179"/>
+      <c r="I74" s="179"/>
+      <c r="J74" s="179"/>
       <c r="K74" s="5"/>
       <c r="L74"/>
     </row>
@@ -4269,17 +4267,17 @@
       <c r="A75" s="141">
         <v>0.77083333333333337</v>
       </c>
-      <c r="B75" s="254" t="s">
-        <v>266</v>
-      </c>
-      <c r="C75" s="254"/>
-      <c r="D75" s="254"/>
-      <c r="E75" s="254"/>
-      <c r="F75" s="254"/>
-      <c r="G75" s="254"/>
-      <c r="H75" s="254"/>
-      <c r="I75" s="254"/>
-      <c r="J75" s="254"/>
+      <c r="B75" s="192" t="s">
+        <v>264</v>
+      </c>
+      <c r="C75" s="192"/>
+      <c r="D75" s="192"/>
+      <c r="E75" s="192"/>
+      <c r="F75" s="192"/>
+      <c r="G75" s="192"/>
+      <c r="H75" s="192"/>
+      <c r="I75" s="192"/>
+      <c r="J75" s="192"/>
       <c r="K75" s="5"/>
     </row>
     <row r="76" spans="1:16" s="1" customFormat="1" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
@@ -4306,9 +4304,6 @@
       <c r="E77" s="97"/>
       <c r="F77" s="97"/>
       <c r="G77" s="97"/>
-      <c r="H77" s="97"/>
-      <c r="I77" s="97"/>
-      <c r="J77" s="97"/>
       <c r="K77" s="22"/>
     </row>
     <row r="78" spans="1:16" s="8" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4326,17 +4321,17 @@
     </row>
     <row r="79" spans="1:16" s="1" customFormat="1" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="12"/>
-      <c r="B79" s="227" t="s">
+      <c r="B79" s="180" t="s">
         <v>65</v>
       </c>
-      <c r="C79" s="227"/>
-      <c r="D79" s="227"/>
-      <c r="E79" s="227"/>
-      <c r="F79" s="227"/>
-      <c r="G79" s="227"/>
-      <c r="H79" s="150"/>
-      <c r="I79" s="150"/>
-      <c r="J79" s="150"/>
+      <c r="C79" s="180"/>
+      <c r="D79" s="180"/>
+      <c r="E79" s="180"/>
+      <c r="F79" s="180"/>
+      <c r="G79" s="180"/>
+      <c r="H79" s="169"/>
+      <c r="I79" s="169"/>
+      <c r="J79" s="169"/>
       <c r="K79" s="5"/>
       <c r="N79" s="10"/>
       <c r="O79" s="10"/>
@@ -4344,35 +4339,35 @@
     </row>
     <row r="80" spans="1:16" s="9" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="14"/>
-      <c r="B80" s="191" t="s">
+      <c r="B80" s="201" t="s">
         <v>203</v>
       </c>
-      <c r="C80" s="192"/>
-      <c r="D80" s="192"/>
-      <c r="E80" s="191" t="s">
+      <c r="C80" s="202"/>
+      <c r="D80" s="202"/>
+      <c r="E80" s="201" t="s">
         <v>204</v>
       </c>
-      <c r="F80" s="192"/>
-      <c r="G80" s="192"/>
-      <c r="H80" s="229"/>
-      <c r="I80" s="230"/>
-      <c r="J80" s="230"/>
+      <c r="F80" s="202"/>
+      <c r="G80" s="202"/>
+      <c r="H80" s="232"/>
+      <c r="I80" s="233"/>
+      <c r="J80" s="233"/>
       <c r="K80" s="23"/>
     </row>
     <row r="81" spans="1:12" s="9" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="14">
         <v>0.38194444444444442</v>
       </c>
-      <c r="B81" s="221" t="s">
+      <c r="B81" s="223" t="s">
         <v>18</v>
       </c>
-      <c r="C81" s="222"/>
-      <c r="D81" s="223"/>
-      <c r="E81" s="247" t="s">
+      <c r="C81" s="224"/>
+      <c r="D81" s="225"/>
+      <c r="E81" s="176" t="s">
         <v>153</v>
       </c>
-      <c r="F81" s="248"/>
-      <c r="G81" s="249"/>
+      <c r="F81" s="177"/>
+      <c r="G81" s="178"/>
       <c r="H81" s="143"/>
       <c r="I81" s="143"/>
       <c r="J81" s="143"/>
@@ -4380,37 +4375,37 @@
     </row>
     <row r="82" spans="1:12" s="9" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="14"/>
-      <c r="B82" s="231" t="s">
+      <c r="B82" s="190" t="s">
         <v>164</v>
       </c>
-      <c r="C82" s="232"/>
-      <c r="D82" s="232"/>
-      <c r="E82" s="188" t="s">
+      <c r="C82" s="191"/>
+      <c r="D82" s="191"/>
+      <c r="E82" s="185" t="s">
         <v>81</v>
       </c>
-      <c r="F82" s="189"/>
-      <c r="G82" s="189"/>
-      <c r="H82" s="255"/>
-      <c r="I82" s="256"/>
-      <c r="J82" s="256"/>
+      <c r="F82" s="186"/>
+      <c r="G82" s="186"/>
+      <c r="H82" s="195"/>
+      <c r="I82" s="196"/>
+      <c r="J82" s="196"/>
       <c r="K82" s="39"/>
       <c r="L82" s="39"/>
     </row>
     <row r="83" spans="1:12" s="9" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="14"/>
-      <c r="B83" s="195" t="s">
+      <c r="B83" s="193" t="s">
         <v>216</v>
       </c>
-      <c r="C83" s="196"/>
-      <c r="D83" s="196"/>
-      <c r="E83" s="177" t="s">
+      <c r="C83" s="194"/>
+      <c r="D83" s="194"/>
+      <c r="E83" s="187" t="s">
         <v>217</v>
       </c>
-      <c r="F83" s="178"/>
-      <c r="G83" s="257"/>
-      <c r="H83" s="197"/>
-      <c r="I83" s="197"/>
-      <c r="J83" s="197"/>
+      <c r="F83" s="188"/>
+      <c r="G83" s="197"/>
+      <c r="H83" s="235"/>
+      <c r="I83" s="235"/>
+      <c r="J83" s="235"/>
       <c r="K83" s="38"/>
       <c r="L83" s="38"/>
     </row>
@@ -4418,13 +4413,13 @@
       <c r="A84" s="14">
         <v>0.38194444444444442</v>
       </c>
-      <c r="B84" s="152">
+      <c r="B84" s="151">
         <v>51</v>
       </c>
-      <c r="C84" s="158" t="s">
+      <c r="C84" s="153" t="s">
         <v>178</v>
       </c>
-      <c r="D84" s="158" t="s">
+      <c r="D84" s="153" t="s">
         <v>179</v>
       </c>
       <c r="E84" s="86">
@@ -4446,13 +4441,13 @@
       <c r="A85" s="14">
         <v>0.40972222222222227</v>
       </c>
-      <c r="B85" s="153">
+      <c r="B85" s="152">
         <v>32</v>
       </c>
-      <c r="C85" s="165" t="s">
+      <c r="C85" s="158" t="s">
         <v>180</v>
       </c>
-      <c r="D85" s="165" t="s">
+      <c r="D85" s="158" t="s">
         <v>181</v>
       </c>
       <c r="E85" s="85">
@@ -4474,14 +4469,14 @@
       <c r="A86" s="14">
         <v>0.4375</v>
       </c>
-      <c r="B86" s="246" t="s">
+      <c r="B86" s="175" t="s">
         <v>219</v>
       </c>
-      <c r="C86" s="246"/>
-      <c r="D86" s="246"/>
-      <c r="E86" s="246"/>
-      <c r="F86" s="246"/>
-      <c r="G86" s="246"/>
+      <c r="C86" s="175"/>
+      <c r="D86" s="175"/>
+      <c r="E86" s="175"/>
+      <c r="F86" s="175"/>
+      <c r="G86" s="175"/>
       <c r="H86" s="144"/>
       <c r="I86" s="144"/>
       <c r="J86" s="144"/>
@@ -4489,54 +4484,54 @@
     </row>
     <row r="87" spans="1:12" s="1" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A87" s="13"/>
-      <c r="B87" s="250" t="s">
+      <c r="B87" s="181" t="s">
         <v>154</v>
       </c>
-      <c r="C87" s="251"/>
-      <c r="D87" s="252"/>
-      <c r="E87" s="253" t="s">
+      <c r="C87" s="182"/>
+      <c r="D87" s="183"/>
+      <c r="E87" s="184" t="s">
         <v>17</v>
       </c>
-      <c r="F87" s="253"/>
-      <c r="G87" s="253"/>
-      <c r="H87" s="219"/>
-      <c r="I87" s="220"/>
-      <c r="J87" s="220"/>
+      <c r="F87" s="184"/>
+      <c r="G87" s="184"/>
+      <c r="H87" s="221"/>
+      <c r="I87" s="222"/>
+      <c r="J87" s="222"/>
       <c r="K87" s="5"/>
     </row>
     <row r="88" spans="1:12" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="13"/>
-      <c r="B88" s="231" t="s">
+      <c r="B88" s="190" t="s">
         <v>165</v>
       </c>
-      <c r="C88" s="232"/>
-      <c r="D88" s="232"/>
-      <c r="E88" s="188" t="s">
+      <c r="C88" s="191"/>
+      <c r="D88" s="191"/>
+      <c r="E88" s="185" t="s">
         <v>82</v>
       </c>
-      <c r="F88" s="189"/>
-      <c r="G88" s="189"/>
-      <c r="H88" s="193"/>
-      <c r="I88" s="194"/>
-      <c r="J88" s="194"/>
+      <c r="F88" s="186"/>
+      <c r="G88" s="186"/>
+      <c r="H88" s="254"/>
+      <c r="I88" s="255"/>
+      <c r="J88" s="255"/>
       <c r="K88" s="39"/>
       <c r="L88" s="39"/>
     </row>
     <row r="89" spans="1:12" s="1" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A89" s="13"/>
-      <c r="B89" s="195" t="s">
+      <c r="B89" s="193" t="s">
         <v>220</v>
       </c>
-      <c r="C89" s="196"/>
-      <c r="D89" s="196"/>
-      <c r="E89" s="177" t="s">
+      <c r="C89" s="194"/>
+      <c r="D89" s="194"/>
+      <c r="E89" s="187" t="s">
         <v>211</v>
       </c>
-      <c r="F89" s="178"/>
-      <c r="G89" s="178"/>
-      <c r="H89" s="200"/>
-      <c r="I89" s="197"/>
-      <c r="J89" s="197"/>
+      <c r="F89" s="188"/>
+      <c r="G89" s="188"/>
+      <c r="H89" s="234"/>
+      <c r="I89" s="235"/>
+      <c r="J89" s="235"/>
       <c r="K89" s="38"/>
       <c r="L89" s="38"/>
     </row>
@@ -4544,13 +4539,13 @@
       <c r="A90" s="14">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B90" s="155">
+      <c r="B90" s="170">
         <v>2</v>
       </c>
-      <c r="C90" s="158" t="s">
+      <c r="C90" s="153" t="s">
         <v>182</v>
       </c>
-      <c r="D90" s="166" t="s">
+      <c r="D90" s="159" t="s">
         <v>183</v>
       </c>
       <c r="E90" s="86">
@@ -4571,14 +4566,14 @@
       <c r="A91" s="14">
         <v>0.4861111111111111</v>
       </c>
-      <c r="B91" s="156">
-        <v>25</v>
-      </c>
-      <c r="C91" s="167" t="s">
-        <v>184</v>
-      </c>
-      <c r="D91" s="168" t="s">
-        <v>185</v>
+      <c r="B91" s="171">
+        <v>21</v>
+      </c>
+      <c r="C91" s="160" t="s">
+        <v>176</v>
+      </c>
+      <c r="D91" s="172" t="s">
+        <v>177</v>
       </c>
       <c r="E91" s="85">
         <v>48</v>
@@ -4598,13 +4593,13 @@
       <c r="A92" s="14">
         <v>0.51388888888888895</v>
       </c>
-      <c r="B92" s="157">
+      <c r="B92" s="168">
         <v>43</v>
       </c>
-      <c r="C92" s="159" t="s">
+      <c r="C92" s="154" t="s">
         <v>186</v>
       </c>
-      <c r="D92" s="169" t="s">
+      <c r="D92" s="162" t="s">
         <v>187</v>
       </c>
       <c r="E92" s="88">
@@ -4624,15 +4619,15 @@
     </row>
     <row r="93" spans="1:12" s="1" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A93" s="14"/>
-      <c r="B93" s="175" t="s">
+      <c r="B93" s="249" t="s">
         <v>202</v>
       </c>
-      <c r="C93" s="175"/>
-      <c r="D93" s="175"/>
-      <c r="E93" s="175"/>
-      <c r="F93" s="175"/>
-      <c r="G93" s="175"/>
-      <c r="H93" s="170"/>
+      <c r="C93" s="249"/>
+      <c r="D93" s="249"/>
+      <c r="E93" s="249"/>
+      <c r="F93" s="249"/>
+      <c r="G93" s="249"/>
+      <c r="H93" s="163"/>
       <c r="I93" s="101"/>
       <c r="J93" s="102"/>
       <c r="K93" s="26"/>
@@ -4642,28 +4637,28 @@
       <c r="A94" s="13">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B94" s="245" t="s">
+      <c r="B94" s="174" t="s">
         <v>1</v>
       </c>
-      <c r="C94" s="245"/>
-      <c r="D94" s="245"/>
-      <c r="E94" s="245"/>
-      <c r="F94" s="245"/>
-      <c r="G94" s="245"/>
+      <c r="C94" s="174"/>
+      <c r="D94" s="174"/>
+      <c r="E94" s="174"/>
+      <c r="F94" s="174"/>
+      <c r="G94" s="174"/>
       <c r="H94" s="145"/>
       <c r="I94" s="145"/>
       <c r="J94" s="145"/>
       <c r="K94" s="25"/>
     </row>
     <row r="95" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B95" s="198" t="s">
+      <c r="B95" s="179" t="s">
         <v>208</v>
       </c>
-      <c r="C95" s="198"/>
-      <c r="D95" s="198"/>
-      <c r="E95" s="198"/>
-      <c r="F95" s="198"/>
-      <c r="G95" s="198"/>
+      <c r="C95" s="179"/>
+      <c r="D95" s="179"/>
+      <c r="E95" s="179"/>
+      <c r="F95" s="179"/>
+      <c r="G95" s="179"/>
       <c r="H95" s="146"/>
       <c r="I95" s="146"/>
       <c r="J95" s="146"/>
@@ -4673,6 +4668,99 @@
     </row>
   </sheetData>
   <mergeCells count="117">
+    <mergeCell ref="B93:G93"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B53:J53"/>
+    <mergeCell ref="M32:O32"/>
+    <mergeCell ref="E58:F59"/>
+    <mergeCell ref="B69:J69"/>
+    <mergeCell ref="M25:O25"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="H30:J30"/>
+    <mergeCell ref="H31:J31"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="H62:J62"/>
+    <mergeCell ref="H64:J64"/>
+    <mergeCell ref="H88:J88"/>
+    <mergeCell ref="B89:D89"/>
+    <mergeCell ref="E88:G88"/>
+    <mergeCell ref="H83:J83"/>
+    <mergeCell ref="B35:J35"/>
+    <mergeCell ref="B28:J28"/>
+    <mergeCell ref="H89:J89"/>
+    <mergeCell ref="B80:D80"/>
+    <mergeCell ref="E80:G80"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="B10:J10"/>
+    <mergeCell ref="B9:J9"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B13:J13"/>
+    <mergeCell ref="B12:J12"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="B17:J17"/>
+    <mergeCell ref="B18:J18"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="B5:J5"/>
+    <mergeCell ref="B11:J11"/>
+    <mergeCell ref="B27:J27"/>
+    <mergeCell ref="B42:J42"/>
+    <mergeCell ref="H87:J87"/>
+    <mergeCell ref="B81:D81"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="B83:D83"/>
+    <mergeCell ref="B25:J25"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B54:J54"/>
+    <mergeCell ref="B55:J55"/>
+    <mergeCell ref="B39:J39"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B61:J61"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="B60:J60"/>
+    <mergeCell ref="H80:J80"/>
+    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="B44:J44"/>
+    <mergeCell ref="B47:J47"/>
+    <mergeCell ref="B29:J29"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B51:J51"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B26:J26"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="B43:J43"/>
+    <mergeCell ref="B40:J40"/>
+    <mergeCell ref="G58:G59"/>
+    <mergeCell ref="H58:I59"/>
+    <mergeCell ref="J58:J59"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="B56:J56"/>
+    <mergeCell ref="B58:C59"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="H57:J57"/>
+    <mergeCell ref="B41:J41"/>
+    <mergeCell ref="B52:J52"/>
+    <mergeCell ref="E45:G45"/>
     <mergeCell ref="B94:G94"/>
     <mergeCell ref="B86:G86"/>
     <mergeCell ref="E81:G81"/>
@@ -4697,99 +4785,6 @@
     <mergeCell ref="E83:G83"/>
     <mergeCell ref="B71:D71"/>
     <mergeCell ref="B88:D88"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B26:J26"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="B43:J43"/>
-    <mergeCell ref="B40:J40"/>
-    <mergeCell ref="G58:G59"/>
-    <mergeCell ref="H58:I59"/>
-    <mergeCell ref="J58:J59"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="B56:J56"/>
-    <mergeCell ref="B58:C59"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="H57:J57"/>
-    <mergeCell ref="B41:J41"/>
-    <mergeCell ref="B52:J52"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="H87:J87"/>
-    <mergeCell ref="B81:D81"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="B83:D83"/>
-    <mergeCell ref="B25:J25"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B54:J54"/>
-    <mergeCell ref="B55:J55"/>
-    <mergeCell ref="B39:J39"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B61:J61"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="B60:J60"/>
-    <mergeCell ref="H80:J80"/>
-    <mergeCell ref="B82:D82"/>
-    <mergeCell ref="B44:J44"/>
-    <mergeCell ref="B47:J47"/>
-    <mergeCell ref="B29:J29"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B51:J51"/>
-    <mergeCell ref="H89:J89"/>
-    <mergeCell ref="B80:D80"/>
-    <mergeCell ref="E80:G80"/>
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="B10:J10"/>
-    <mergeCell ref="B9:J9"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B13:J13"/>
-    <mergeCell ref="B12:J12"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="B17:J17"/>
-    <mergeCell ref="B18:J18"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="B5:J5"/>
-    <mergeCell ref="B11:J11"/>
-    <mergeCell ref="B27:J27"/>
-    <mergeCell ref="B42:J42"/>
-    <mergeCell ref="B93:G93"/>
-    <mergeCell ref="M20:O20"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B53:J53"/>
-    <mergeCell ref="M32:O32"/>
-    <mergeCell ref="E58:F59"/>
-    <mergeCell ref="B69:J69"/>
-    <mergeCell ref="M25:O25"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="H30:J30"/>
-    <mergeCell ref="H31:J31"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="M23:O23"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="E62:G62"/>
-    <mergeCell ref="H62:J62"/>
-    <mergeCell ref="H64:J64"/>
-    <mergeCell ref="H88:J88"/>
-    <mergeCell ref="B89:D89"/>
-    <mergeCell ref="E88:G88"/>
-    <mergeCell ref="H83:J83"/>
-    <mergeCell ref="B35:J35"/>
-    <mergeCell ref="B28:J28"/>
   </mergeCells>
   <phoneticPr fontId="22" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -4825,10 +4820,10 @@
       <c r="F3" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="264" t="s">
+      <c r="G3" s="287" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="264"/>
+      <c r="H3" s="287"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" s="49">
@@ -4843,10 +4838,10 @@
       <c r="F4" s="49">
         <v>44734</v>
       </c>
-      <c r="G4" s="265">
+      <c r="G4" s="288">
         <v>44735</v>
       </c>
-      <c r="H4" s="265"/>
+      <c r="H4" s="288"/>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="50">
@@ -4866,7 +4861,7 @@
       </c>
       <c r="B6" s="50"/>
       <c r="C6" s="50"/>
-      <c r="D6" s="282" t="s">
+      <c r="D6" s="261" t="s">
         <v>158</v>
       </c>
       <c r="E6" s="50"/>
@@ -4880,7 +4875,7 @@
       </c>
       <c r="B7" s="50"/>
       <c r="C7" s="50"/>
-      <c r="D7" s="283"/>
+      <c r="D7" s="262"/>
       <c r="E7" s="50"/>
       <c r="F7" s="50"/>
       <c r="G7" s="50"/>
@@ -4892,7 +4887,7 @@
       </c>
       <c r="B8" s="50"/>
       <c r="C8" s="50"/>
-      <c r="D8" s="283"/>
+      <c r="D8" s="262"/>
       <c r="E8" s="50"/>
       <c r="F8" s="50"/>
       <c r="G8" s="50"/>
@@ -4904,13 +4899,13 @@
       </c>
       <c r="B9" s="50"/>
       <c r="C9" s="50"/>
-      <c r="D9" s="283"/>
+      <c r="D9" s="262"/>
       <c r="E9" s="50"/>
       <c r="F9" s="50"/>
-      <c r="G9" s="266" t="s">
+      <c r="G9" s="275" t="s">
         <v>53</v>
       </c>
-      <c r="H9" s="269" t="s">
+      <c r="H9" s="267" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4920,15 +4915,15 @@
       </c>
       <c r="B10" s="50"/>
       <c r="C10" s="50"/>
-      <c r="D10" s="283"/>
-      <c r="E10" s="282" t="s">
+      <c r="D10" s="262"/>
+      <c r="E10" s="261" t="s">
         <v>160</v>
       </c>
-      <c r="F10" s="282" t="s">
+      <c r="F10" s="261" t="s">
         <v>160</v>
       </c>
-      <c r="G10" s="267"/>
-      <c r="H10" s="270"/>
+      <c r="G10" s="276"/>
+      <c r="H10" s="268"/>
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="50">
@@ -4936,11 +4931,11 @@
       </c>
       <c r="B11" s="50"/>
       <c r="C11" s="50"/>
-      <c r="D11" s="284"/>
-      <c r="E11" s="283"/>
-      <c r="F11" s="283"/>
-      <c r="G11" s="267"/>
-      <c r="H11" s="270"/>
+      <c r="D11" s="263"/>
+      <c r="E11" s="262"/>
+      <c r="F11" s="262"/>
+      <c r="G11" s="276"/>
+      <c r="H11" s="268"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="50">
@@ -4948,13 +4943,13 @@
       </c>
       <c r="B12" s="50"/>
       <c r="C12" s="50"/>
-      <c r="D12" s="287" t="s">
+      <c r="D12" s="264" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="284"/>
-      <c r="F12" s="284"/>
-      <c r="G12" s="267"/>
-      <c r="H12" s="270"/>
+      <c r="E12" s="263"/>
+      <c r="F12" s="263"/>
+      <c r="G12" s="276"/>
+      <c r="H12" s="268"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="50">
@@ -4962,15 +4957,15 @@
       </c>
       <c r="B13" s="50"/>
       <c r="C13" s="50"/>
-      <c r="D13" s="288"/>
-      <c r="E13" s="285" t="s">
+      <c r="D13" s="265"/>
+      <c r="E13" s="259" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="285" t="s">
+      <c r="F13" s="259" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="267"/>
-      <c r="H13" s="270"/>
+      <c r="G13" s="276"/>
+      <c r="H13" s="268"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="50">
@@ -4978,11 +4973,11 @@
       </c>
       <c r="B14" s="50"/>
       <c r="C14" s="50"/>
-      <c r="D14" s="288"/>
-      <c r="E14" s="286"/>
-      <c r="F14" s="286"/>
-      <c r="G14" s="268"/>
-      <c r="H14" s="271"/>
+      <c r="D14" s="265"/>
+      <c r="E14" s="260"/>
+      <c r="F14" s="260"/>
+      <c r="G14" s="277"/>
+      <c r="H14" s="269"/>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="50">
@@ -4990,17 +4985,17 @@
       </c>
       <c r="B15" s="50"/>
       <c r="C15" s="50"/>
-      <c r="D15" s="289"/>
-      <c r="E15" s="287" t="s">
+      <c r="D15" s="266"/>
+      <c r="E15" s="264" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="287" t="s">
+      <c r="F15" s="264" t="s">
         <v>5</v>
       </c>
-      <c r="G15" s="272" t="s">
+      <c r="G15" s="289" t="s">
         <v>11</v>
       </c>
-      <c r="H15" s="273"/>
+      <c r="H15" s="290"/>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="50">
@@ -5008,13 +5003,13 @@
       </c>
       <c r="B16" s="50"/>
       <c r="C16" s="50"/>
-      <c r="D16" s="285" t="s">
+      <c r="D16" s="259" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="288"/>
-      <c r="F16" s="288"/>
-      <c r="G16" s="274"/>
-      <c r="H16" s="275"/>
+      <c r="E16" s="265"/>
+      <c r="F16" s="265"/>
+      <c r="G16" s="291"/>
+      <c r="H16" s="292"/>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="50">
@@ -5022,13 +5017,13 @@
       </c>
       <c r="B17" s="50"/>
       <c r="C17" s="50"/>
-      <c r="D17" s="286"/>
-      <c r="E17" s="288"/>
-      <c r="F17" s="288"/>
-      <c r="G17" s="266" t="s">
+      <c r="D17" s="260"/>
+      <c r="E17" s="265"/>
+      <c r="F17" s="265"/>
+      <c r="G17" s="275" t="s">
         <v>54</v>
       </c>
-      <c r="H17" s="269" t="s">
+      <c r="H17" s="267" t="s">
         <v>31</v>
       </c>
     </row>
@@ -5038,13 +5033,13 @@
       </c>
       <c r="B18" s="50"/>
       <c r="C18" s="50"/>
-      <c r="D18" s="269" t="s">
+      <c r="D18" s="267" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="288"/>
-      <c r="F18" s="288"/>
-      <c r="G18" s="267"/>
-      <c r="H18" s="270"/>
+      <c r="E18" s="265"/>
+      <c r="F18" s="265"/>
+      <c r="G18" s="276"/>
+      <c r="H18" s="268"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="50">
@@ -5052,11 +5047,11 @@
       </c>
       <c r="B19" s="50"/>
       <c r="C19" s="50"/>
-      <c r="D19" s="270"/>
-      <c r="E19" s="288"/>
-      <c r="F19" s="288"/>
-      <c r="G19" s="267"/>
-      <c r="H19" s="270"/>
+      <c r="D19" s="268"/>
+      <c r="E19" s="265"/>
+      <c r="F19" s="265"/>
+      <c r="G19" s="276"/>
+      <c r="H19" s="268"/>
     </row>
     <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="50">
@@ -5064,11 +5059,11 @@
       </c>
       <c r="B20" s="50"/>
       <c r="C20" s="50"/>
-      <c r="D20" s="270"/>
-      <c r="E20" s="288"/>
-      <c r="F20" s="288"/>
-      <c r="G20" s="267"/>
-      <c r="H20" s="270"/>
+      <c r="D20" s="268"/>
+      <c r="E20" s="265"/>
+      <c r="F20" s="265"/>
+      <c r="G20" s="276"/>
+      <c r="H20" s="268"/>
     </row>
     <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="50">
@@ -5076,11 +5071,11 @@
       </c>
       <c r="B21" s="50"/>
       <c r="C21" s="50"/>
-      <c r="D21" s="270"/>
-      <c r="E21" s="288"/>
-      <c r="F21" s="288"/>
-      <c r="G21" s="267"/>
-      <c r="H21" s="270"/>
+      <c r="D21" s="268"/>
+      <c r="E21" s="265"/>
+      <c r="F21" s="265"/>
+      <c r="G21" s="276"/>
+      <c r="H21" s="268"/>
     </row>
     <row r="22" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="50">
@@ -5088,11 +5083,11 @@
       </c>
       <c r="B22" s="50"/>
       <c r="C22" s="50"/>
-      <c r="D22" s="270"/>
-      <c r="E22" s="289"/>
-      <c r="F22" s="289"/>
-      <c r="G22" s="267"/>
-      <c r="H22" s="270"/>
+      <c r="D22" s="268"/>
+      <c r="E22" s="266"/>
+      <c r="F22" s="266"/>
+      <c r="G22" s="276"/>
+      <c r="H22" s="268"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="50">
@@ -5100,15 +5095,15 @@
       </c>
       <c r="B23" s="50"/>
       <c r="C23" s="50"/>
-      <c r="D23" s="270"/>
-      <c r="E23" s="290" t="s">
+      <c r="D23" s="268"/>
+      <c r="E23" s="270" t="s">
         <v>6</v>
       </c>
-      <c r="F23" s="290" t="s">
+      <c r="F23" s="270" t="s">
         <v>6</v>
       </c>
-      <c r="G23" s="267"/>
-      <c r="H23" s="270"/>
+      <c r="G23" s="276"/>
+      <c r="H23" s="268"/>
     </row>
     <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="50">
@@ -5116,11 +5111,11 @@
       </c>
       <c r="B24" s="50"/>
       <c r="C24" s="50"/>
-      <c r="D24" s="270"/>
-      <c r="E24" s="291"/>
-      <c r="F24" s="291"/>
-      <c r="G24" s="268"/>
-      <c r="H24" s="271"/>
+      <c r="D24" s="268"/>
+      <c r="E24" s="271"/>
+      <c r="F24" s="271"/>
+      <c r="G24" s="277"/>
+      <c r="H24" s="269"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="50">
@@ -5128,13 +5123,13 @@
       </c>
       <c r="B25" s="50"/>
       <c r="C25" s="50"/>
-      <c r="D25" s="271"/>
-      <c r="E25" s="291"/>
-      <c r="F25" s="291"/>
-      <c r="G25" s="276" t="s">
+      <c r="D25" s="269"/>
+      <c r="E25" s="271"/>
+      <c r="F25" s="271"/>
+      <c r="G25" s="293" t="s">
         <v>56</v>
       </c>
-      <c r="H25" s="277"/>
+      <c r="H25" s="294"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="50">
@@ -5142,13 +5137,13 @@
       </c>
       <c r="B26" s="50"/>
       <c r="C26" s="50"/>
-      <c r="D26" s="290" t="s">
+      <c r="D26" s="270" t="s">
         <v>6</v>
       </c>
-      <c r="E26" s="292"/>
-      <c r="F26" s="292"/>
-      <c r="G26" s="278"/>
-      <c r="H26" s="279"/>
+      <c r="E26" s="272"/>
+      <c r="F26" s="272"/>
+      <c r="G26" s="295"/>
+      <c r="H26" s="296"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="50">
@@ -5156,15 +5151,15 @@
       </c>
       <c r="B27" s="50"/>
       <c r="C27" s="50"/>
-      <c r="D27" s="291"/>
+      <c r="D27" s="271"/>
       <c r="E27" s="50"/>
-      <c r="F27" s="269" t="s">
+      <c r="F27" s="267" t="s">
         <v>9</v>
       </c>
-      <c r="G27" s="258" t="s">
+      <c r="G27" s="281" t="s">
         <v>6</v>
       </c>
-      <c r="H27" s="259"/>
+      <c r="H27" s="282"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="50">
@@ -5172,11 +5167,11 @@
       </c>
       <c r="B28" s="50"/>
       <c r="C28" s="50"/>
-      <c r="D28" s="291"/>
+      <c r="D28" s="271"/>
       <c r="E28" s="50"/>
-      <c r="F28" s="270"/>
-      <c r="G28" s="260"/>
-      <c r="H28" s="261"/>
+      <c r="F28" s="268"/>
+      <c r="G28" s="283"/>
+      <c r="H28" s="284"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="50">
@@ -5184,11 +5179,11 @@
       </c>
       <c r="B29" s="50"/>
       <c r="C29" s="50"/>
-      <c r="D29" s="292"/>
+      <c r="D29" s="272"/>
       <c r="E29" s="50"/>
-      <c r="F29" s="270"/>
-      <c r="G29" s="260"/>
-      <c r="H29" s="261"/>
+      <c r="F29" s="268"/>
+      <c r="G29" s="283"/>
+      <c r="H29" s="284"/>
     </row>
     <row r="30" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="50">
@@ -5196,13 +5191,13 @@
       </c>
       <c r="B30" s="50"/>
       <c r="C30" s="50"/>
-      <c r="D30" s="282" t="s">
+      <c r="D30" s="261" t="s">
         <v>159</v>
       </c>
       <c r="E30" s="50"/>
-      <c r="F30" s="270"/>
-      <c r="G30" s="262"/>
-      <c r="H30" s="263"/>
+      <c r="F30" s="268"/>
+      <c r="G30" s="285"/>
+      <c r="H30" s="286"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="50">
@@ -5210,9 +5205,9 @@
       </c>
       <c r="B31" s="50"/>
       <c r="C31" s="50"/>
-      <c r="D31" s="283"/>
+      <c r="D31" s="262"/>
       <c r="E31" s="50"/>
-      <c r="F31" s="270"/>
+      <c r="F31" s="268"/>
       <c r="G31" s="50"/>
       <c r="H31" s="50"/>
     </row>
@@ -5222,9 +5217,9 @@
       </c>
       <c r="B32" s="50"/>
       <c r="C32" s="50"/>
-      <c r="D32" s="283"/>
+      <c r="D32" s="262"/>
       <c r="E32" s="50"/>
-      <c r="F32" s="270"/>
+      <c r="F32" s="268"/>
       <c r="G32" s="50"/>
       <c r="H32" s="50"/>
     </row>
@@ -5234,9 +5229,9 @@
       </c>
       <c r="B33" s="50"/>
       <c r="C33" s="50"/>
-      <c r="D33" s="284"/>
+      <c r="D33" s="263"/>
       <c r="E33" s="50"/>
-      <c r="F33" s="270"/>
+      <c r="F33" s="268"/>
       <c r="G33" s="50"/>
       <c r="H33" s="50"/>
     </row>
@@ -5246,11 +5241,11 @@
       </c>
       <c r="B34" s="50"/>
       <c r="C34" s="50"/>
-      <c r="D34" s="285" t="s">
+      <c r="D34" s="259" t="s">
         <v>11</v>
       </c>
       <c r="E34" s="50"/>
-      <c r="F34" s="271"/>
+      <c r="F34" s="269"/>
       <c r="G34" s="50"/>
       <c r="H34" s="50"/>
     </row>
@@ -5260,9 +5255,9 @@
       </c>
       <c r="B35" s="50"/>
       <c r="C35" s="50"/>
-      <c r="D35" s="286"/>
+      <c r="D35" s="260"/>
       <c r="E35" s="50"/>
-      <c r="F35" s="285" t="s">
+      <c r="F35" s="259" t="s">
         <v>11</v>
       </c>
       <c r="G35" s="50"/>
@@ -5272,17 +5267,17 @@
       <c r="A36" s="50">
         <v>0.65625</v>
       </c>
-      <c r="D36" s="269" t="s">
+      <c r="D36" s="267" t="s">
         <v>8</v>
       </c>
-      <c r="F36" s="286"/>
+      <c r="F36" s="260"/>
     </row>
     <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="50">
         <v>0.66666666666666696</v>
       </c>
-      <c r="D37" s="270"/>
-      <c r="F37" s="266" t="s">
+      <c r="D37" s="268"/>
+      <c r="F37" s="275" t="s">
         <v>10</v>
       </c>
     </row>
@@ -5290,42 +5285,42 @@
       <c r="A38" s="50">
         <v>0.67708333333333337</v>
       </c>
-      <c r="D38" s="270"/>
-      <c r="F38" s="267"/>
+      <c r="D38" s="268"/>
+      <c r="F38" s="276"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="50">
         <v>0.6875</v>
       </c>
-      <c r="D39" s="270"/>
-      <c r="F39" s="267"/>
+      <c r="D39" s="268"/>
+      <c r="F39" s="276"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="50">
         <v>0.69791666666666663</v>
       </c>
-      <c r="D40" s="270"/>
-      <c r="F40" s="267"/>
+      <c r="D40" s="268"/>
+      <c r="F40" s="276"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="50">
         <v>0.70833333333333404</v>
       </c>
-      <c r="D41" s="270"/>
-      <c r="F41" s="267"/>
+      <c r="D41" s="268"/>
+      <c r="F41" s="276"/>
     </row>
     <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="50">
         <v>0.71875</v>
       </c>
-      <c r="D42" s="270"/>
-      <c r="F42" s="268"/>
+      <c r="D42" s="268"/>
+      <c r="F42" s="277"/>
     </row>
     <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="50">
         <v>0.72916666666666663</v>
       </c>
-      <c r="D43" s="271"/>
+      <c r="D43" s="269"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="50">
@@ -5346,10 +5341,10 @@
       <c r="A47" s="50">
         <v>0.77083333333333337</v>
       </c>
-      <c r="C47" s="296" t="s">
+      <c r="C47" s="256" t="s">
         <v>58</v>
       </c>
-      <c r="F47" s="293" t="s">
+      <c r="F47" s="278" t="s">
         <v>57</v>
       </c>
     </row>
@@ -5357,90 +5352,90 @@
       <c r="A48" s="50">
         <v>0.78125</v>
       </c>
-      <c r="C48" s="297"/>
-      <c r="F48" s="294"/>
+      <c r="C48" s="257"/>
+      <c r="F48" s="279"/>
     </row>
     <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="50">
         <v>0.79166666666666663</v>
       </c>
-      <c r="C49" s="297"/>
-      <c r="F49" s="294"/>
+      <c r="C49" s="257"/>
+      <c r="F49" s="279"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="50">
         <v>0.80208333333333337</v>
       </c>
-      <c r="C50" s="298"/>
-      <c r="F50" s="294"/>
+      <c r="C50" s="258"/>
+      <c r="F50" s="279"/>
     </row>
     <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="50">
         <v>0.8125</v>
       </c>
-      <c r="F51" s="294"/>
+      <c r="F51" s="279"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="50">
         <v>0.82291666666666663</v>
       </c>
-      <c r="F52" s="294"/>
+      <c r="F52" s="279"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="50">
         <v>0.83333333333333337</v>
       </c>
-      <c r="F53" s="294"/>
+      <c r="F53" s="279"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="50">
         <v>0.84375</v>
       </c>
-      <c r="F54" s="294"/>
+      <c r="F54" s="279"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="50">
         <v>0.85416666666666663</v>
       </c>
-      <c r="F55" s="294"/>
+      <c r="F55" s="279"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="50">
         <v>0.86458333333333337</v>
       </c>
-      <c r="F56" s="294"/>
+      <c r="F56" s="279"/>
     </row>
     <row r="57" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="50">
         <v>0.875</v>
       </c>
-      <c r="F57" s="295"/>
+      <c r="F57" s="280"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D59" s="280" t="s">
+      <c r="D59" s="273" t="s">
         <v>12</v>
       </c>
-      <c r="E59" s="280"/>
-      <c r="F59" s="280"/>
+      <c r="E59" s="273"/>
+      <c r="F59" s="273"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D60" s="281" t="s">
+      <c r="D60" s="274" t="s">
         <v>13</v>
       </c>
-      <c r="E60" s="281"/>
-      <c r="F60" s="281"/>
+      <c r="E60" s="274"/>
+      <c r="F60" s="274"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="C47:C50"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="D6:D11"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="D18:D25"/>
-    <mergeCell ref="D26:D29"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="D36:D43"/>
+    <mergeCell ref="G27:H30"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G17:G24"/>
+    <mergeCell ref="H17:H24"/>
+    <mergeCell ref="G9:G14"/>
+    <mergeCell ref="H9:H14"/>
+    <mergeCell ref="G15:H16"/>
+    <mergeCell ref="G25:H26"/>
     <mergeCell ref="D59:F59"/>
     <mergeCell ref="D60:F60"/>
     <mergeCell ref="E10:E12"/>
@@ -5455,15 +5450,15 @@
     <mergeCell ref="F35:F36"/>
     <mergeCell ref="F37:F42"/>
     <mergeCell ref="F47:F57"/>
-    <mergeCell ref="G27:H30"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G17:G24"/>
-    <mergeCell ref="H17:H24"/>
-    <mergeCell ref="G9:G14"/>
-    <mergeCell ref="H9:H14"/>
-    <mergeCell ref="G15:H16"/>
-    <mergeCell ref="G25:H26"/>
+    <mergeCell ref="C47:C50"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D6:D11"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="D18:D25"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="D36:D43"/>
   </mergeCells>
   <phoneticPr fontId="22" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5721,27 +5716,27 @@
       <c r="B1" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="299" t="s">
+      <c r="C1" s="297" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="299"/>
-      <c r="E1" s="299"/>
-      <c r="F1" s="299"/>
-      <c r="G1" s="299"/>
-      <c r="H1" s="299"/>
-      <c r="I1" s="299"/>
-      <c r="J1" s="299"/>
-      <c r="K1" s="299"/>
-      <c r="L1" s="299"/>
-      <c r="M1" s="299"/>
+      <c r="D1" s="297"/>
+      <c r="E1" s="297"/>
+      <c r="F1" s="297"/>
+      <c r="G1" s="297"/>
+      <c r="H1" s="297"/>
+      <c r="I1" s="297"/>
+      <c r="J1" s="297"/>
+      <c r="K1" s="297"/>
+      <c r="L1" s="297"/>
+      <c r="M1" s="297"/>
       <c r="N1" s="64"/>
       <c r="O1" s="64"/>
-      <c r="P1" s="300" t="s">
+      <c r="P1" s="298" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="300"/>
-      <c r="R1" s="300"/>
-      <c r="S1" s="300"/>
+      <c r="Q1" s="298"/>
+      <c r="R1" s="298"/>
+      <c r="S1" s="298"/>
       <c r="T1" s="67"/>
       <c r="U1" s="67"/>
       <c r="V1" s="67"/>
@@ -6428,27 +6423,27 @@
       <c r="B1" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="299" t="s">
+      <c r="C1" s="297" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="299"/>
-      <c r="E1" s="299"/>
-      <c r="F1" s="299"/>
-      <c r="G1" s="299"/>
-      <c r="H1" s="299"/>
-      <c r="I1" s="299"/>
-      <c r="J1" s="299"/>
-      <c r="K1" s="299"/>
-      <c r="L1" s="299"/>
-      <c r="M1" s="299"/>
-      <c r="N1" s="151"/>
-      <c r="O1" s="151"/>
-      <c r="P1" s="300" t="s">
+      <c r="D1" s="297"/>
+      <c r="E1" s="297"/>
+      <c r="F1" s="297"/>
+      <c r="G1" s="297"/>
+      <c r="H1" s="297"/>
+      <c r="I1" s="297"/>
+      <c r="J1" s="297"/>
+      <c r="K1" s="297"/>
+      <c r="L1" s="297"/>
+      <c r="M1" s="297"/>
+      <c r="N1" s="150"/>
+      <c r="O1" s="150"/>
+      <c r="P1" s="298" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="300"/>
-      <c r="R1" s="300"/>
-      <c r="S1" s="300"/>
+      <c r="Q1" s="298"/>
+      <c r="R1" s="298"/>
+      <c r="S1" s="298"/>
       <c r="T1" s="67"/>
       <c r="U1" s="67"/>
       <c r="V1" s="67"/>

</xml_diff>